<commit_message>
updating string sources in xlsx
</commit_message>
<xml_diff>
--- a/sources/daadario/strings.xlsx
+++ b/sources/daadario/strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hido/Development/github.com/haisamido/msdb/sources/daadario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{77A9071D-F853-964C-93BD-AEC17AB86D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D064E21D-3A89-8B4F-A0D8-415246CF7D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41120" yWindow="500" windowWidth="28380" windowHeight="16520" activeTab="2"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="127">
   <si>
     <t>Classical Guitar</t>
   </si>
@@ -209,76 +209,211 @@
     <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-j4302-pro-arte-nylon-classical-guitar-single-string-light-tension-first-string-1031/</t>
   </si>
   <si>
-    <t>Single Clear Nylon 0275/J43 1st Light Tension</t>
-  </si>
-  <si>
-    <t>Single Clear Nylon 0397/J43 3rd Light Tension</t>
-  </si>
-  <si>
-    <t>Single Clear Nylon 0317/J43 2nd Light Tension</t>
-  </si>
-  <si>
-    <t>Single Silver Wound 028/J43 4th Light Tension</t>
-  </si>
-  <si>
-    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-j9999-pro-arte-nylon-classical-guitar-single-string-light-tension-first-string-1032/</t>
-  </si>
-  <si>
-    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-j9999-pro-arte-nylon-classical-guitar-single-string-light-tension-first-string-1033/</t>
-  </si>
-  <si>
-    <t>Single Silver Wound 033/J43 5th Light Tension</t>
-  </si>
-  <si>
-    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-j9999-pro-arte-nylon-classical-guitar-single-string-light-tension-first-string-1034/</t>
-  </si>
-  <si>
-    <t>Single Silver Wound 042/J43 6th Light Tension</t>
-  </si>
-  <si>
-    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-j9999-pro-arte-nylon-classical-guitar-single-string-light-tension-first-string-1030/</t>
-  </si>
-  <si>
-    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-j9999-pro-arte-nylon-classical-guitar-single-string-light-tension-first-string-1031/</t>
-  </si>
-  <si>
-    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-j9999-pro-arte-nylon-classical-guitar-single-string-light-tension-first-string-1029/</t>
-  </si>
-  <si>
-    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1029/</t>
-  </si>
-  <si>
-    <t>https://www.daddario.com/products/guitar/single-strings/classical-trebles/pro-arte-trebles/item/daddario-j4301-pro-arte-nylon-classical-guitar-single-string-light-tension-first-string-1035/</t>
-  </si>
-  <si>
     <t>EJ47</t>
   </si>
   <si>
     <t>J4704</t>
   </si>
   <si>
-    <t>https://www.daddario.com/products/guitar/single-strings/classical-trebles/pro-arte-trebles/item/daddario-j4301-pro-arte-nylon-classical-guitar-single-string-light-tension-first-string-1036/</t>
-  </si>
-  <si>
-    <t>https://www.daddario.com/products/guitar/single-strings/classical-trebles/pro-arte-trebles/item/daddario-j4301-pro-arte-nylon-classical-guitar-single-string-light-tension-first-string-1037/</t>
-  </si>
-  <si>
     <t>J4705</t>
   </si>
   <si>
-    <t>https://www.daddario.com/products/guitar/single-strings/classical-trebles/pro-arte-trebles/item/daddario-j4301-pro-arte-nylon-classical-guitar-single-string-light-tension-first-string-1038/</t>
-  </si>
-  <si>
     <t>J4706</t>
   </si>
   <si>
-    <t>Single 80/20 Bronze Wound 043/J47 6th Normal Tension</t>
-  </si>
-  <si>
-    <t>Single 80/20 Bronze Wound 035/J47 5th Normal Tension</t>
-  </si>
-  <si>
-    <t>Single 80/20 Bronze Wound 029/J47 4th Normal Tension</t>
+    <t>EJ48</t>
+  </si>
+  <si>
+    <t>80/20 Bronze Wrap, Nylon Core, Clear Nylon Trebles</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1029</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1030</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1031</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1032</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1033</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1034</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1042</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1043</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1044</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1036</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1037</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1038</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1039</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1040</t>
+  </si>
+  <si>
+    <t>Silver Plated Wrap, Nylon Core, Clear Nylon Trebles</t>
+  </si>
+  <si>
+    <t>EJ45</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Clear Nylon 0275/J43 1st Light Tension</t>
+  </si>
+  <si>
+    <t>Clear Nylon 0317/J43 2nd Light Tension</t>
+  </si>
+  <si>
+    <t>Clear Nylon 0397/J43 3rd Light Tension</t>
+  </si>
+  <si>
+    <t>Silver Wound 028/J43 4th Light Tension</t>
+  </si>
+  <si>
+    <t>Silver Wound 033/J43 5th Light Tension</t>
+  </si>
+  <si>
+    <t>Silver Wound 042/J43 6th Light Tension</t>
+  </si>
+  <si>
+    <t>80/20 Bronze Wound 029/J47 4th Normal Tension</t>
+  </si>
+  <si>
+    <t>80/20 Bronze Wound 035/J47 5th Normal Tension</t>
+  </si>
+  <si>
+    <t>80/20 Bronze Wound 043/J47 6th Normal Tension</t>
+  </si>
+  <si>
+    <t>Silver Wound 029/J45 4th Normal Tension</t>
+  </si>
+  <si>
+    <t>Silver Wound 035/J45 5th Normal Tension</t>
+  </si>
+  <si>
+    <t>Silver Wound 043/J45 6th Normal Tension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1035 </t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1020</t>
+  </si>
+  <si>
+    <t>EXP46</t>
+  </si>
+  <si>
+    <t>Hard Tension</t>
+  </si>
+  <si>
+    <t>EXP4604</t>
+  </si>
+  <si>
+    <t>.030 4TH String Hard Tension</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1021</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1022</t>
+  </si>
+  <si>
+    <t>.036 5TH String Hard Tension</t>
+  </si>
+  <si>
+    <t>EXP4605</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1023</t>
+  </si>
+  <si>
+    <t>.044 6TH String Hard Tension</t>
+  </si>
+  <si>
+    <t>EXP4606</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1024</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1025</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1026</t>
+  </si>
+  <si>
+    <t>EXP44</t>
+  </si>
+  <si>
+    <t>Extra Hard Tension</t>
+  </si>
+  <si>
+    <t>.030 4TH String Extra Hard Tension</t>
+  </si>
+  <si>
+    <t>EXP4404</t>
+  </si>
+  <si>
+    <t>.036 5TH String Extra Hard Tension</t>
+  </si>
+  <si>
+    <t>EXP4405</t>
+  </si>
+  <si>
+    <t>.047 6TH String Extra Hard Tension</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1027</t>
+  </si>
+  <si>
+    <t>EXP4406</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1028</t>
+  </si>
+  <si>
+    <t>EJ43</t>
+  </si>
+  <si>
+    <t>strebles</t>
+  </si>
+  <si>
+    <t>basses</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1041</t>
+  </si>
+  <si>
+    <t>Silver Plated Wrap, Nylon Core, Clear Nylon</t>
+  </si>
+  <si>
+    <t>EJ45-3D</t>
+  </si>
+  <si>
+    <t>sets</t>
   </si>
 </sst>
 </file>
@@ -2245,144 +2380,523 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D25"/>
+  <dimension ref="B2:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="143.1640625" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2">
+        <v>1028</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B3" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="E3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3">
+        <v>1029</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B4" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="E4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4">
+        <v>1030</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" t="s">
-        <v>59</v>
+        <v>66</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="D5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B7" t="s">
+      <c r="E5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5">
+        <v>1032</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6">
+        <v>1032</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B7" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7">
+        <v>1033</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8">
+        <v>1034</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B11" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11">
+        <v>1036</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12">
+        <v>1037</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13">
+        <v>1038</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17">
+        <v>1042</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18">
+        <v>1043</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B19" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19">
+        <v>1044</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B22" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22">
+        <v>1021</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23">
+        <v>1022</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24">
+        <v>1023</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B25" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B26" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26">
+        <v>1025</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B27" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27">
+        <v>1026</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28">
+        <v>1027</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B8" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B22" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B23" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="E31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B25" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>78</v>
+      <c r="F31">
+        <v>1039</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B23" r:id="rId4"/>
-    <hyperlink ref="B25" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B19" r:id="rId3"/>
+    <hyperlink ref="B11" r:id="rId4"/>
+    <hyperlink ref="B12" r:id="rId5"/>
+    <hyperlink ref="B13" r:id="rId6"/>
+    <hyperlink ref="B31" r:id="rId7"/>
+    <hyperlink ref="B15" r:id="rId8"/>
+    <hyperlink ref="B3" r:id="rId9"/>
+    <hyperlink ref="B4" r:id="rId10"/>
+    <hyperlink ref="B6" r:id="rId11"/>
+    <hyperlink ref="B8" r:id="rId12"/>
+    <hyperlink ref="B10" r:id="rId13"/>
+    <hyperlink ref="B22" r:id="rId14"/>
+    <hyperlink ref="B25" r:id="rId15"/>
+    <hyperlink ref="B26" r:id="rId16"/>
+    <hyperlink ref="B27" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
some additional string content
</commit_message>
<xml_diff>
--- a/sources/daadario/strings.xlsx
+++ b/sources/daadario/strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hido/Development/github.com/haisamido/msdb/sources/daadario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D064E21D-3A89-8B4F-A0D8-415246CF7D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{39FF875B-B779-6241-A5EB-CCA665787CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41120" yWindow="500" windowWidth="28380" windowHeight="16520" activeTab="2"/>
+    <workbookView xWindow="41480" yWindow="500" windowWidth="28380" windowHeight="16520" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="daadario" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="138">
   <si>
     <t>Classical Guitar</t>
   </si>
@@ -414,6 +414,39 @@
   </si>
   <si>
     <t>sets</t>
+  </si>
+  <si>
+    <t>grep '&lt;span id="product-subtitle-text"&gt;'</t>
+  </si>
+  <si>
+    <t>cat daddario-1000 | grep '&lt;span id="product-code"&gt;'</t>
+  </si>
+  <si>
+    <t>cat daddario-1000 | grep '{"event":"productDetails"'</t>
+  </si>
+  <si>
+    <t>wget -q -O - https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1001 | grep '&lt;span id="product-code"&gt;'</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1000</t>
+  </si>
+  <si>
+    <t>Clear Nylon 0416/J44 3rd Extra-Hard Tension</t>
+  </si>
+  <si>
+    <t>J4403</t>
+  </si>
+  <si>
+    <t>treble</t>
+  </si>
+  <si>
+    <t>https://www.daddario.com/products/guitar/single-strings/classical-basses/pro-arte-basses/item/daddario-1001</t>
+  </si>
+  <si>
+    <t>Silver Plated Wrap, Composite Core, Clear Nylon Trebles</t>
+  </si>
+  <si>
+    <t>EJ44C</t>
   </si>
 </sst>
 </file>
@@ -2380,16 +2413,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G31"/>
+  <dimension ref="B2:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="87.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
@@ -2397,424 +2430,343 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4">
+        <v>1001</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B10" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F2">
-        <v>1028</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B3" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3">
-        <v>1029</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B4" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4">
-        <v>1030</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B5" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5">
-        <v>1032</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B6" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F6">
-        <v>1032</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B7" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7">
-        <v>1033</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B8" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8">
-        <v>1034</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B10" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F10">
-        <v>1035</v>
+        <v>1028</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B11" s="5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>82</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>81</v>
       </c>
       <c r="F11">
-        <v>1036</v>
+        <v>1029</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B12" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>60</v>
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>81</v>
       </c>
       <c r="F12">
-        <v>1037</v>
+        <v>1030</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B13" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>61</v>
+        <v>84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>81</v>
       </c>
       <c r="F13">
-        <v>1038</v>
+        <v>1032</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14">
+        <v>1032</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" t="s">
-        <v>78</v>
+        <v>68</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15">
+        <v>1033</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16">
+        <v>1034</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B18" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F15">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B16" t="s">
-        <v>123</v>
-      </c>
-      <c r="C16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F16">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17">
-        <v>1042</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="F18">
-        <v>1043</v>
+        <v>1035</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>122</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B19" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>81</v>
       </c>
       <c r="F19">
-        <v>1044</v>
+        <v>1036</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>122</v>
       </c>
     </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B20" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20">
+        <v>1037</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B21" t="s">
-        <v>95</v>
+      <c r="B21" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21">
+        <v>1038</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F21">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B22" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22">
-        <v>1021</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="F23">
-        <v>1022</v>
+        <v>1040</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>122</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>105</v>
+        <v>123</v>
+      </c>
+      <c r="C24" t="s">
+        <v>124</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24">
+        <v>1041</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F24">
-        <v>1023</v>
-      </c>
-      <c r="G24" s="1" t="s">
+      <c r="F25">
+        <v>1042</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B25" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25">
-        <v>1024</v>
-      </c>
-    </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B26" s="5" t="s">
-        <v>108</v>
+      <c r="B26" t="s">
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>113</v>
+        <v>21</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>81</v>
       </c>
       <c r="F26">
-        <v>1025</v>
+        <v>1043</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>122</v>
@@ -2822,81 +2774,244 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B27" s="5" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>115</v>
+        <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>81</v>
       </c>
       <c r="F27">
-        <v>1026</v>
+        <v>1044</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B28" t="s">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29">
+        <v>1020</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B30" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30">
+        <v>1021</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31">
+        <v>1022</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B32" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32">
+        <v>1023</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B33" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33">
+        <v>1024</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B34" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F34">
+        <v>1025</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B35" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35">
+        <v>1026</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B36" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F28">
+      <c r="F36">
         <v>1027</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B31" s="5" t="s">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B38" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C38" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F31">
+      <c r="F38">
         <v>1039</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B42" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B43" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B44" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B47" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B19" r:id="rId3"/>
-    <hyperlink ref="B11" r:id="rId4"/>
-    <hyperlink ref="B12" r:id="rId5"/>
-    <hyperlink ref="B13" r:id="rId6"/>
-    <hyperlink ref="B31" r:id="rId7"/>
-    <hyperlink ref="B15" r:id="rId8"/>
-    <hyperlink ref="B3" r:id="rId9"/>
-    <hyperlink ref="B4" r:id="rId10"/>
-    <hyperlink ref="B6" r:id="rId11"/>
-    <hyperlink ref="B8" r:id="rId12"/>
-    <hyperlink ref="B10" r:id="rId13"/>
-    <hyperlink ref="B22" r:id="rId14"/>
-    <hyperlink ref="B25" r:id="rId15"/>
-    <hyperlink ref="B26" r:id="rId16"/>
-    <hyperlink ref="B27" r:id="rId17"/>
+    <hyperlink ref="B15" r:id="rId1"/>
+    <hyperlink ref="B13" r:id="rId2"/>
+    <hyperlink ref="B27" r:id="rId3"/>
+    <hyperlink ref="B19" r:id="rId4"/>
+    <hyperlink ref="B20" r:id="rId5"/>
+    <hyperlink ref="B21" r:id="rId6"/>
+    <hyperlink ref="B38" r:id="rId7"/>
+    <hyperlink ref="B23" r:id="rId8"/>
+    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B12" r:id="rId10"/>
+    <hyperlink ref="B14" r:id="rId11"/>
+    <hyperlink ref="B16" r:id="rId12"/>
+    <hyperlink ref="B18" r:id="rId13"/>
+    <hyperlink ref="B30" r:id="rId14"/>
+    <hyperlink ref="B33" r:id="rId15"/>
+    <hyperlink ref="B34" r:id="rId16"/>
+    <hyperlink ref="B35" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
added more strings to spreadsheet
</commit_message>
<xml_diff>
--- a/sources/daadario/strings.xlsx
+++ b/sources/daadario/strings.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hido/Development/github.com/haisamido/msdb/sources/daadario/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hido/Development/github.com/haisamido/organology/sources/daadario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{39FF875B-B779-6241-A5EB-CCA665787CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF989AF-1416-4A45-933B-8E450431F8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41480" yWindow="500" windowWidth="28380" windowHeight="16520" activeTab="2"/>
+    <workbookView xWindow="35340" yWindow="500" windowWidth="28380" windowHeight="16520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="daadario" sheetId="1" r:id="rId1"/>
-    <sheet name="note ranges" sheetId="2" r:id="rId2"/>
-    <sheet name="sources" sheetId="3" r:id="rId3"/>
+    <sheet name="main" sheetId="4" r:id="rId1"/>
+    <sheet name="daadario" sheetId="1" r:id="rId2"/>
+    <sheet name="note ranges" sheetId="2" r:id="rId3"/>
+    <sheet name="sources" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="195">
   <si>
     <t>Classical Guitar</t>
   </si>
@@ -447,13 +448,187 @@
   </si>
   <si>
     <t>EJ44C</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>4,5,6</t>
+  </si>
+  <si>
+    <t>J4401</t>
+  </si>
+  <si>
+    <t>J4402</t>
+  </si>
+  <si>
+    <t>J4501</t>
+  </si>
+  <si>
+    <t>J4502</t>
+  </si>
+  <si>
+    <t>J4503</t>
+  </si>
+  <si>
+    <t>J4601</t>
+  </si>
+  <si>
+    <t>J4602</t>
+  </si>
+  <si>
+    <t>J4603</t>
+  </si>
+  <si>
+    <t>J4701</t>
+  </si>
+  <si>
+    <t>J4702</t>
+  </si>
+  <si>
+    <t>J4703</t>
+  </si>
+  <si>
+    <t>J4801</t>
+  </si>
+  <si>
+    <t>J4802</t>
+  </si>
+  <si>
+    <t>J4803</t>
+  </si>
+  <si>
+    <t>J5101</t>
+  </si>
+  <si>
+    <t>J5102</t>
+  </si>
+  <si>
+    <t>J5103</t>
+  </si>
+  <si>
+    <t>Laser Select clear nylon</t>
+  </si>
+  <si>
+    <t>laser select black nylon</t>
+  </si>
+  <si>
+    <t>J4901</t>
+  </si>
+  <si>
+    <t>J4902</t>
+  </si>
+  <si>
+    <t>J4903</t>
+  </si>
+  <si>
+    <t>J5001</t>
+  </si>
+  <si>
+    <t>J5002</t>
+  </si>
+  <si>
+    <t>J5003</t>
+  </si>
+  <si>
+    <t>rectified clear nylon</t>
+  </si>
+  <si>
+    <t>J2801</t>
+  </si>
+  <si>
+    <t>J2802</t>
+  </si>
+  <si>
+    <t>J2803</t>
+  </si>
+  <si>
+    <t>J2901</t>
+  </si>
+  <si>
+    <t>J2902</t>
+  </si>
+  <si>
+    <t>J2903</t>
+  </si>
+  <si>
+    <t>J3001</t>
+  </si>
+  <si>
+    <t>J3002</t>
+  </si>
+  <si>
+    <t>J3003</t>
+  </si>
+  <si>
+    <t>J3101</t>
+  </si>
+  <si>
+    <t>J3102</t>
+  </si>
+  <si>
+    <t>J3103</t>
+  </si>
+  <si>
+    <t>D’Addario Classic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.00000000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -472,6 +647,11 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -497,15 +677,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -820,20 +1001,437 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:S34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7371A15C-E6E0-EA40-BA40-999FDB30E53F}">
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1.0203E-4</v>
+      </c>
+      <c r="F2" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="G2" s="3">
+        <v>11.7</v>
+      </c>
+      <c r="H2" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="I2" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J2" s="3">
+        <v>6.6</v>
+      </c>
+      <c r="K2" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="L2" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="M2" s="3">
+        <v>3.7</v>
+      </c>
+      <c r="N2" s="1" t="str">
+        <f>MID(D2,3,1)</f>
+        <v>3</v>
+      </c>
+      <c r="O2" s="1" t="str">
+        <f>CONCATENATE("E",MID(D2,1,3))</f>
+        <v>EJ43</v>
+      </c>
+      <c r="P2" s="1" t="str">
+        <f>MID(D2,5,1)</f>
+        <v>4</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.5347000000000001E-4</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3">
+        <v>17.7</v>
+      </c>
+      <c r="H3" s="3">
+        <v>15.8</v>
+      </c>
+      <c r="I3" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="J3" s="3">
+        <v>9.9</v>
+      </c>
+      <c r="K3" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="L3" s="3">
+        <v>7</v>
+      </c>
+      <c r="M3" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="N3" s="1" t="str">
+        <f t="shared" ref="N3:N4" si="0">MID(D3,3,1)</f>
+        <v>3</v>
+      </c>
+      <c r="O3" s="1" t="str">
+        <f t="shared" ref="O3:O4" si="1">CONCATENATE("E",MID(D3,1,3))</f>
+        <v>EJ43</v>
+      </c>
+      <c r="P3" s="1" t="str">
+        <f t="shared" ref="P3:P4" si="2">MID(D3,5,1)</f>
+        <v>5</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.8881000000000002E-4</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="3">
+        <v>23.5</v>
+      </c>
+      <c r="J4" s="3">
+        <v>18.7</v>
+      </c>
+      <c r="K4" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="L4" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="M4" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>EJ43</v>
+      </c>
+      <c r="P4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2.0239999999999999E-5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G9" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="H9" s="3">
+        <v>11.8</v>
+      </c>
+      <c r="I9" s="3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J9" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K9" s="3">
+        <v>6.6</v>
+      </c>
+      <c r="L9" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="M9" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="N9" s="1" t="str">
+        <f>MID(D9,3,1)</f>
+        <v>3</v>
+      </c>
+      <c r="O9" s="1" t="str">
+        <f>CONCATENATE("E",MID(D9,1,3))</f>
+        <v>EJ43</v>
+      </c>
+      <c r="P9" s="1" t="str">
+        <f>MID(D9,5,1)</f>
+        <v>1</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.7290000000000001E-5</v>
+      </c>
+      <c r="F10" s="3">
+        <v>22.4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>20</v>
+      </c>
+      <c r="H10" s="3">
+        <v>15.8</v>
+      </c>
+      <c r="I10" s="3">
+        <v>12.6</v>
+      </c>
+      <c r="J10" s="3">
+        <v>11.2</v>
+      </c>
+      <c r="K10" s="3">
+        <v>8.9</v>
+      </c>
+      <c r="L10" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="N10" s="1" t="str">
+        <f t="shared" ref="N10:N11" si="3">MID(D10,3,1)</f>
+        <v>3</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f t="shared" ref="O10:O11" si="4">CONCATENATE("E",MID(D10,1,3))</f>
+        <v>EJ43</v>
+      </c>
+      <c r="P10" s="1" t="str">
+        <f t="shared" ref="P10:P11" si="5">MID(D10,5,1)</f>
+        <v>2</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4.5250000000000002E-5</v>
+      </c>
+      <c r="F11" s="3">
+        <v>37.1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>33.1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>26.3</v>
+      </c>
+      <c r="I11" s="3">
+        <v>20.8</v>
+      </c>
+      <c r="J11" s="3">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="K11" s="3">
+        <v>14.7</v>
+      </c>
+      <c r="L11" s="3">
+        <v>11.7</v>
+      </c>
+      <c r="M11" s="3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="N11" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="O11" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>EJ43</v>
+      </c>
+      <c r="P11" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S10" r:id="rId1" xr:uid="{F385F0E0-E94F-BD4A-A860-A13A72375E42}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A5:S75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="6" customWidth="1"/>
     <col min="6" max="13" width="7.83203125" style="1" customWidth="1"/>
     <col min="14" max="15" width="8.83203125" style="1"/>
     <col min="16" max="16" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -843,11 +1441,8 @@
     <col min="20" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="D4" s="3"/>
-    </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -856,10 +1451,10 @@
       <c r="C5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -897,7 +1492,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -906,34 +1501,34 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6">
         <v>1.0203E-4</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="1">
         <v>14.8</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="1">
         <v>11.7</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="1">
         <v>10.5</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="1">
         <v>8.3000000000000007</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="1">
         <v>6.6</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="1">
         <v>5.2</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="1">
         <v>4.7</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="1">
         <v>3.7</v>
       </c>
       <c r="N6" s="1" t="str">
@@ -953,7 +1548,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -962,34 +1557,34 @@
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="6">
         <v>1.5347000000000001E-4</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="1">
         <v>17.7</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="1">
         <v>15.8</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="1">
         <v>12.5</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="1">
         <v>9.9</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="1">
         <v>7.9</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="1">
         <v>7</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="1">
         <v>5.6</v>
       </c>
       <c r="N7" s="1" t="str">
@@ -1009,7 +1604,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1018,34 +1613,34 @@
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="6">
         <v>2.8881000000000002E-4</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="1">
         <v>23.5</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="1">
         <v>18.7</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="1">
         <v>14.8</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="1">
         <v>13.2</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="1">
         <v>10.5</v>
       </c>
       <c r="N8" s="1" t="str">
@@ -1065,7 +1660,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1074,34 +1669,34 @@
       <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="6">
         <v>1.1237E-4</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="1">
         <v>16.3</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="1">
         <v>12.9</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="1">
         <v>11.5</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="1">
         <v>9.1999999999999993</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="1">
         <v>7.3</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="1">
         <v>5.8</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="1">
         <v>4.0999999999999996</v>
       </c>
       <c r="N9" s="1" t="str">
@@ -1121,7 +1716,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1130,34 +1725,34 @@
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="6">
         <v>1.9521E-4</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="1">
         <v>20</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="1">
         <v>15.9</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="1">
         <v>12.6</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="1">
         <v>10</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="1">
         <v>8.9</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="1">
         <v>7.1</v>
       </c>
       <c r="N10" s="1" t="str">
@@ -1177,7 +1772,7 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1186,34 +1781,34 @@
       <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="6">
         <v>3.4351E-4</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="1">
         <v>17.600000000000001</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="1">
         <v>15.7</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="1">
         <v>12.5</v>
       </c>
       <c r="N11" s="1" t="str">
@@ -1233,7 +1828,7 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1242,34 +1837,34 @@
       <c r="C12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="6">
         <v>1.0754E-4</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="1">
         <v>15.6</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="1">
         <v>12.4</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="1">
         <v>11</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="1">
         <v>8.8000000000000007</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="1">
         <v>7</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="1">
         <v>5.5</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="1">
         <v>4.9000000000000004</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="1">
         <v>3.9</v>
       </c>
       <c r="N12" s="1" t="str">
@@ -1286,7 +1881,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1295,34 +1890,34 @@
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="6">
         <v>1.8416E-4</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="1">
         <v>18.899999999999999</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="1">
         <v>15</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="1">
         <v>11.9</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="1">
         <v>9.4</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="1">
         <v>8.4</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="1">
         <v>6.7</v>
       </c>
       <c r="N13" s="1" t="str">
@@ -1339,7 +1934,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1348,34 +1943,34 @@
       <c r="C14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="6">
         <v>3.0632000000000001E-4</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="1">
         <v>19.8</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="1">
         <v>15.7</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="1">
         <v>14</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="1">
         <v>11.1</v>
       </c>
       <c r="N14" s="1" t="str">
@@ -1392,7 +1987,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1401,34 +1996,34 @@
       <c r="C15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="6">
         <v>1.1237E-4</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="1">
         <v>16.3</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="1">
         <v>12.9</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="1">
         <v>11.5</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="1">
         <v>9.1999999999999993</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="1">
         <v>7.3</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="1">
         <v>5.8</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="1">
         <v>4.0999999999999996</v>
       </c>
       <c r="N15" s="1" t="str">
@@ -1448,7 +2043,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1457,34 +2052,34 @@
       <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="6">
         <v>1.9521E-4</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="1">
         <v>20</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="1">
         <v>15.9</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="1">
         <v>12.6</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="1">
         <v>10</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="1">
         <v>8.9</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="1">
         <v>7.1</v>
       </c>
       <c r="N16" s="1" t="str">
@@ -1504,7 +2099,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1513,34 +2108,34 @@
       <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="6">
         <v>3.1725999999999998E-4</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="1">
         <v>20.5</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="1">
         <v>16.3</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="1">
         <v>14.5</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="1">
         <v>11.5</v>
       </c>
       <c r="N17" s="1" t="str">
@@ -1560,7 +2155,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1569,34 +2164,34 @@
       <c r="C18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="6">
         <v>1.0754E-4</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="1">
         <v>15.6</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="1">
         <v>12.4</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="1">
         <v>11</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="1">
         <v>8.8000000000000007</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="1">
         <v>7</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="1">
         <v>5.5</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="1">
         <v>4.9000000000000004</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18" s="1">
         <v>3.9</v>
       </c>
       <c r="N18" s="1" t="str">
@@ -1616,7 +2211,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1625,34 +2220,34 @@
       <c r="C19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="6">
         <v>1.8416E-4</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="1">
         <v>18.899999999999999</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="1">
         <v>15</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="1">
         <v>11.9</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="1">
         <v>9.4</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19" s="1">
         <v>8.4</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M19" s="1">
         <v>6.7</v>
       </c>
       <c r="N19" s="1" t="str">
@@ -1672,7 +2267,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1681,34 +2276,34 @@
       <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="6">
         <v>3.0632000000000001E-4</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="1">
         <v>19.8</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="1">
         <v>15.7</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="1">
         <v>14</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20" s="1">
         <v>11.1</v>
       </c>
       <c r="N20" s="1" t="str">
@@ -1728,7 +2323,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1737,34 +2332,34 @@
       <c r="C21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="6">
         <v>1.1237E-4</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="1">
         <v>16.3</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="1">
         <v>12.9</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="1">
         <v>11.5</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="1">
         <v>9.1999999999999993</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="1">
         <v>7.3</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="1">
         <v>5.8</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21" s="1">
         <v>4.0999999999999996</v>
       </c>
       <c r="N21" s="1" t="str">
@@ -1787,7 +2382,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -1796,34 +2391,34 @@
       <c r="C22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="6">
         <v>1.9521E-4</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="1">
         <v>20</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="1">
         <v>15.9</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="1">
         <v>12.6</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="1">
         <v>10</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="1">
         <v>8.9</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M22" s="1">
         <v>7.1</v>
       </c>
       <c r="N22" s="1" t="str">
@@ -1846,7 +2441,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1855,34 +2450,34 @@
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="6">
         <v>3.1725999999999998E-4</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="1">
         <v>20.5</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="1">
         <v>16.3</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="1">
         <v>14.5</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M23" s="1">
         <v>11.5</v>
       </c>
       <c r="N23" s="1" t="str">
@@ -1904,65 +2499,34 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-    </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="D27" s="1"/>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L27" s="4" t="s">
+      <c r="L27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="M27" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1974,31 +2538,31 @@
       <c r="D28" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="6">
         <v>2.0239999999999999E-5</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="1">
         <v>16.600000000000001</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="1">
         <v>14.8</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="1">
         <v>11.8</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="1">
         <v>9.3000000000000007</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="1">
         <v>8.3000000000000007</v>
       </c>
-      <c r="K28" s="4">
+      <c r="K28" s="1">
         <v>6.6</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="1">
         <v>5.2</v>
       </c>
-      <c r="M28" s="4">
+      <c r="M28" s="1">
         <v>4.2</v>
       </c>
       <c r="N28" s="1" t="str">
@@ -2021,7 +2585,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2033,31 +2597,31 @@
       <c r="D29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="6">
         <v>2.7290000000000001E-5</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="1">
         <v>22.4</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="1">
         <v>20</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="1">
         <v>15.8</v>
       </c>
-      <c r="I29" s="4">
+      <c r="I29" s="1">
         <v>12.6</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29" s="1">
         <v>11.2</v>
       </c>
-      <c r="K29" s="4">
+      <c r="K29" s="1">
         <v>8.9</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29" s="1">
         <v>7.1</v>
       </c>
-      <c r="M29" s="4">
+      <c r="M29" s="1">
         <v>5.6</v>
       </c>
       <c r="N29" s="1" t="str">
@@ -2075,12 +2639,12 @@
       <c r="R29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="S29" s="5" t="s">
+      <c r="S29" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2092,31 +2656,31 @@
       <c r="D30" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="6">
         <v>4.5250000000000002E-5</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="1">
         <v>37.1</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="1">
         <v>33.1</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="1">
         <v>26.3</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="1">
         <v>20.8</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J30" s="1">
         <v>18.600000000000001</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K30" s="1">
         <v>14.7</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="1">
         <v>11.7</v>
       </c>
-      <c r="M30" s="4">
+      <c r="M30" s="1">
         <v>9.3000000000000007</v>
       </c>
       <c r="N30" s="1" t="str">
@@ -2134,274 +2698,2355 @@
       <c r="R30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="S30" s="5" t="s">
+      <c r="S30" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="F31" s="4" t="s">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="E33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="6">
+        <v>2.0239999999999999E-5</v>
+      </c>
+      <c r="F34" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G34" s="1">
+        <v>14.8</v>
+      </c>
+      <c r="H34" s="1">
+        <v>11.8</v>
+      </c>
+      <c r="I34" s="1">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J34" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K34" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="L34" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="M34" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="N34" s="1" t="str">
+        <f>MID(D34,3,1)</f>
+        <v>3</v>
+      </c>
+      <c r="O34" s="1" t="str">
+        <f t="shared" ref="O34:O54" si="6">CONCATENATE("E",MID(D34,1,3))</f>
+        <v>EJ43</v>
+      </c>
+      <c r="P34" s="1" t="str">
+        <f>MID(D34,5,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="6">
+        <v>2.7290000000000001E-5</v>
+      </c>
+      <c r="F35" s="1">
+        <v>22.4</v>
+      </c>
+      <c r="G35" s="1">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="I35" s="1">
+        <v>12.6</v>
+      </c>
+      <c r="J35" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="K35" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="L35" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="M35" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="N35" s="1" t="str">
+        <f t="shared" ref="N35:N54" si="7">MID(D35,3,1)</f>
+        <v>3</v>
+      </c>
+      <c r="O35" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ43</v>
+      </c>
+      <c r="P35" s="1" t="str">
+        <f t="shared" ref="P35:P54" si="8">MID(D35,5,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="6">
+        <v>4.5250000000000002E-5</v>
+      </c>
+      <c r="F36" s="1">
+        <v>37.1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>33.1</v>
+      </c>
+      <c r="H36" s="1">
+        <v>26.3</v>
+      </c>
+      <c r="I36" s="1">
+        <v>20.8</v>
+      </c>
+      <c r="J36" s="1">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="K36" s="1">
+        <v>14.7</v>
+      </c>
+      <c r="L36" s="1">
+        <v>11.7</v>
+      </c>
+      <c r="M36" s="1">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="N36" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="O36" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ43</v>
+      </c>
+      <c r="P36" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" s="6">
+        <v>2.243E-5</v>
+      </c>
+      <c r="F37" s="1">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="G37" s="1">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="H37" s="1">
+        <v>13</v>
+      </c>
+      <c r="I37" s="1">
+        <v>10.3</v>
+      </c>
+      <c r="J37" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="K37" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="L37" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="M37" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="N37" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="O37" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ44</v>
+      </c>
+      <c r="P37" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38" s="6">
+        <v>3.046E-5</v>
+      </c>
+      <c r="F38" s="1">
+        <v>25</v>
+      </c>
+      <c r="G38" s="1">
+        <v>22.3</v>
+      </c>
+      <c r="H38" s="1">
+        <v>17.7</v>
+      </c>
+      <c r="I38" s="1">
+        <v>14</v>
+      </c>
+      <c r="J38" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="K38" s="1">
+        <v>9.9</v>
+      </c>
+      <c r="L38" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="M38" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="N38" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="O38" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ44</v>
+      </c>
+      <c r="P38" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E39" s="6">
+        <v>4.9889999999999998E-5</v>
+      </c>
+      <c r="F39" s="1">
+        <v>40.9</v>
+      </c>
+      <c r="G39" s="1">
+        <v>36.5</v>
+      </c>
+      <c r="H39" s="1">
+        <v>29</v>
+      </c>
+      <c r="I39" s="1">
+        <v>23</v>
+      </c>
+      <c r="J39" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="K39" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="L39" s="1">
+        <v>12.9</v>
+      </c>
+      <c r="M39" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="N39" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="O39" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ44</v>
+      </c>
+      <c r="P39" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E40" s="6">
+        <v>2.092E-5</v>
+      </c>
+      <c r="F40" s="1">
+        <v>17.2</v>
+      </c>
+      <c r="G40" s="1">
+        <v>15.3</v>
+      </c>
+      <c r="H40" s="1">
+        <v>12.1</v>
+      </c>
+      <c r="I40" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="J40" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="K40" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="L40" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="M40" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="N40" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="O40" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ45</v>
+      </c>
+      <c r="P40" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E41" s="6">
+        <v>2.8269999999999999E-5</v>
+      </c>
+      <c r="F41" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="G41" s="1">
+        <v>20.7</v>
+      </c>
+      <c r="H41" s="1">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="I41" s="1">
+        <v>13</v>
+      </c>
+      <c r="J41" s="1">
+        <v>11.6</v>
+      </c>
+      <c r="K41" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L41" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="M41" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="N41" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="O41" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ45</v>
+      </c>
+      <c r="P41" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E42" s="6">
+        <v>4.6789999999999998E-5</v>
+      </c>
+      <c r="F42" s="1">
+        <v>38.4</v>
+      </c>
+      <c r="G42" s="1">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="H42" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="I42" s="1">
+        <v>21.6</v>
+      </c>
+      <c r="J42" s="1">
+        <v>19.2</v>
+      </c>
+      <c r="K42" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="L42" s="1">
+        <v>12.1</v>
+      </c>
+      <c r="M42" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="N42" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="O42" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ45</v>
+      </c>
+      <c r="P42" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E43" s="6">
+        <v>2.1610000000000001E-5</v>
+      </c>
+      <c r="F43" s="1">
+        <v>17.7</v>
+      </c>
+      <c r="G43" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="H43" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="I43" s="1">
+        <v>10</v>
+      </c>
+      <c r="J43" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="K43" s="1">
+        <v>7</v>
+      </c>
+      <c r="L43" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="M43" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N43" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="O43" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ46</v>
+      </c>
+      <c r="P43" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E44" s="6">
+        <v>2.9240000000000001E-5</v>
+      </c>
+      <c r="F44" s="1">
+        <v>24</v>
+      </c>
+      <c r="G44" s="1">
+        <v>21.4</v>
+      </c>
+      <c r="H44" s="1">
+        <v>17</v>
+      </c>
+      <c r="I44" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="J44" s="1">
+        <v>12</v>
+      </c>
+      <c r="K44" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="L44" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="M44" s="1">
+        <v>6</v>
+      </c>
+      <c r="N44" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="O44" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ46</v>
+      </c>
+      <c r="P44" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E45" s="6">
+        <v>4.795E-5</v>
+      </c>
+      <c r="F45" s="1">
+        <v>39.4</v>
+      </c>
+      <c r="G45" s="1">
+        <v>35.1</v>
+      </c>
+      <c r="H45" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="I45" s="1">
+        <v>22.1</v>
+      </c>
+      <c r="J45" s="1">
+        <v>19.7</v>
+      </c>
+      <c r="K45" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="L45" s="1">
+        <v>12.4</v>
+      </c>
+      <c r="M45" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="N45" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="O45" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ46</v>
+      </c>
+      <c r="P45" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E46" s="6">
+        <v>2.092E-5</v>
+      </c>
+      <c r="F46" s="1">
+        <v>17.2</v>
+      </c>
+      <c r="G46" s="1">
+        <v>15.3</v>
+      </c>
+      <c r="H46" s="1">
+        <v>12.1</v>
+      </c>
+      <c r="I46" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="J46" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="K46" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="L46" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="M46" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="N46" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="O46" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ47</v>
+      </c>
+      <c r="P46" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E47" s="6">
+        <v>2.8269999999999999E-5</v>
+      </c>
+      <c r="F47" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="G47" s="1">
+        <v>20.7</v>
+      </c>
+      <c r="H47" s="1">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="I47" s="1">
+        <v>13</v>
+      </c>
+      <c r="J47" s="1">
+        <v>11.6</v>
+      </c>
+      <c r="K47" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L47" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="M47" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="N47" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="O47" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ47</v>
+      </c>
+      <c r="P47" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E48" s="6">
+        <v>4.6789999999999998E-5</v>
+      </c>
+      <c r="F48" s="1">
+        <v>38.4</v>
+      </c>
+      <c r="G48" s="1">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="H48" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="I48" s="1">
+        <v>21.6</v>
+      </c>
+      <c r="J48" s="1">
+        <v>19.2</v>
+      </c>
+      <c r="K48" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="L48" s="1">
+        <v>12.1</v>
+      </c>
+      <c r="M48" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="N48" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="O48" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ47</v>
+      </c>
+      <c r="P48" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A49" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E49" s="6">
+        <v>2.1610000000000001E-5</v>
+      </c>
+      <c r="F49" s="1">
+        <v>17.7</v>
+      </c>
+      <c r="G49" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="H49" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="I49" s="1">
+        <v>10</v>
+      </c>
+      <c r="J49" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="K49" s="1">
+        <v>7</v>
+      </c>
+      <c r="L49" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="M49" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N49" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="O49" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ48</v>
+      </c>
+      <c r="P49" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E50" s="6">
+        <v>2.9240000000000001E-5</v>
+      </c>
+      <c r="F50" s="1">
+        <v>24</v>
+      </c>
+      <c r="G50" s="1">
+        <v>21.4</v>
+      </c>
+      <c r="H50" s="1">
+        <v>17</v>
+      </c>
+      <c r="I50" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="J50" s="1">
+        <v>12</v>
+      </c>
+      <c r="K50" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="L50" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="M50" s="1">
+        <v>6</v>
+      </c>
+      <c r="N50" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="O50" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ48</v>
+      </c>
+      <c r="P50" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E51" s="6">
+        <v>4.795E-5</v>
+      </c>
+      <c r="F51" s="1">
+        <v>39.4</v>
+      </c>
+      <c r="G51" s="1">
+        <v>35.1</v>
+      </c>
+      <c r="H51" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="I51" s="1">
+        <v>22.1</v>
+      </c>
+      <c r="J51" s="1">
+        <v>19.7</v>
+      </c>
+      <c r="K51" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="L51" s="1">
+        <v>12.4</v>
+      </c>
+      <c r="M51" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="N51" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="O51" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ48</v>
+      </c>
+      <c r="P51" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E52" s="6">
+        <v>2.1610000000000001E-5</v>
+      </c>
+      <c r="F52" s="1">
+        <v>17.7</v>
+      </c>
+      <c r="G52" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="H52" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="I52" s="1">
+        <v>10</v>
+      </c>
+      <c r="J52" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="K52" s="1">
+        <v>7</v>
+      </c>
+      <c r="L52" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="M52" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N52" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="O52" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ51</v>
+      </c>
+      <c r="P52" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E53" s="6">
+        <v>2.9240000000000001E-5</v>
+      </c>
+      <c r="F53" s="1">
+        <v>24</v>
+      </c>
+      <c r="G53" s="1">
+        <v>21.4</v>
+      </c>
+      <c r="H53" s="1">
+        <v>17</v>
+      </c>
+      <c r="I53" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="J53" s="1">
+        <v>12</v>
+      </c>
+      <c r="K53" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="L53" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="M53" s="1">
+        <v>6</v>
+      </c>
+      <c r="N53" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="O53" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ51</v>
+      </c>
+      <c r="P53" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E54" s="6">
+        <v>4.795E-5</v>
+      </c>
+      <c r="F54" s="1">
+        <v>39.4</v>
+      </c>
+      <c r="G54" s="1">
+        <v>35.1</v>
+      </c>
+      <c r="H54" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="I54" s="1">
+        <v>22.1</v>
+      </c>
+      <c r="J54" s="1">
+        <v>19.7</v>
+      </c>
+      <c r="K54" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="L54" s="1">
+        <v>12.4</v>
+      </c>
+      <c r="M54" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="N54" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="O54" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>EJ51</v>
+      </c>
+      <c r="P54" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A57" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E57" s="6">
+        <v>2.092E-5</v>
+      </c>
+      <c r="F57" s="1">
+        <v>17.2</v>
+      </c>
+      <c r="G57" s="1">
+        <v>15.3</v>
+      </c>
+      <c r="H57" s="1">
+        <v>12.1</v>
+      </c>
+      <c r="I57" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="J57" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="K57" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="L57" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="M57" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="N57" s="1" t="str">
+        <f t="shared" ref="N57" si="9">MID(D57,3,1)</f>
         <v>9</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="O57" s="1" t="str">
+        <f t="shared" ref="O57" si="10">CONCATENATE("E",MID(D57,1,3))</f>
+        <v>EJ49</v>
+      </c>
+      <c r="P57" s="1" t="str">
+        <f t="shared" ref="P57" si="11">MID(D57,5,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E58" s="6">
+        <v>2.8269999999999999E-5</v>
+      </c>
+      <c r="F58" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="G58" s="1">
+        <v>20.7</v>
+      </c>
+      <c r="H58" s="1">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="I58" s="1">
+        <v>13</v>
+      </c>
+      <c r="J58" s="1">
+        <v>11.6</v>
+      </c>
+      <c r="K58" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L58" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="M58" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="N58" s="1" t="str">
+        <f t="shared" ref="N58:N62" si="12">MID(D58,3,1)</f>
+        <v>9</v>
+      </c>
+      <c r="O58" s="1" t="str">
+        <f t="shared" ref="O58:O62" si="13">CONCATENATE("E",MID(D58,1,3))</f>
+        <v>EJ49</v>
+      </c>
+      <c r="P58" s="1" t="str">
+        <f t="shared" ref="P58:P62" si="14">MID(D58,5,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E59" s="6">
+        <v>4.6789999999999998E-5</v>
+      </c>
+      <c r="F59" s="1">
+        <v>38.4</v>
+      </c>
+      <c r="G59" s="1">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="H59" s="1">
+        <v>27.2</v>
+      </c>
+      <c r="I59" s="1">
+        <v>21.6</v>
+      </c>
+      <c r="J59" s="1">
+        <v>19.2</v>
+      </c>
+      <c r="K59" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="L59" s="1">
+        <v>12.1</v>
+      </c>
+      <c r="M59" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="N59" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="O59" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>EJ49</v>
+      </c>
+      <c r="P59" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E60" s="6">
+        <v>2.1610000000000001E-5</v>
+      </c>
+      <c r="F60" s="1">
+        <v>17.7</v>
+      </c>
+      <c r="G60" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="H60" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="I60" s="1">
         <v>10</v>
       </c>
-      <c r="L31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M31" s="4" t="s">
+      <c r="J60" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="K60" s="1">
+        <v>7</v>
+      </c>
+      <c r="L60" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="M60" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N60" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O60" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>EJ50</v>
+      </c>
+      <c r="P60" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E61" s="6">
+        <v>2.9240000000000001E-5</v>
+      </c>
+      <c r="F61" s="1">
+        <v>24</v>
+      </c>
+      <c r="G61" s="1">
+        <v>21.4</v>
+      </c>
+      <c r="H61" s="1">
+        <v>17</v>
+      </c>
+      <c r="I61" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="J61" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="K61" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="L61" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="M61" s="1">
+        <v>6</v>
+      </c>
+      <c r="N61" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O61" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>EJ50</v>
+      </c>
+      <c r="P61" s="1" t="str">
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="1">
-        <v>1.0203E-4</v>
-      </c>
-      <c r="F32" s="4">
-        <v>14.8</v>
-      </c>
-      <c r="G32" s="4">
-        <v>11.7</v>
-      </c>
-      <c r="H32" s="4">
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E62" s="6">
+        <v>4.795E-5</v>
+      </c>
+      <c r="F62" s="1">
+        <v>39.4</v>
+      </c>
+      <c r="G62" s="1">
+        <v>35.1</v>
+      </c>
+      <c r="H62" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="I62" s="1">
+        <v>22.1</v>
+      </c>
+      <c r="J62" s="1">
+        <v>19.7</v>
+      </c>
+      <c r="K62" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="L62" s="1">
+        <v>12.4</v>
+      </c>
+      <c r="M62" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="N62" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="O62" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>EJ50</v>
+      </c>
+      <c r="P62" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E64" s="6">
+        <v>2.065E-5</v>
+      </c>
+      <c r="F64" s="1">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G64" s="1">
+        <v>15.1</v>
+      </c>
+      <c r="H64" s="1">
+        <v>12</v>
+      </c>
+      <c r="I64" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="J64" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="K64" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="L64" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="M64" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="N64" s="1" t="str">
+        <f t="shared" ref="N64" si="15">MID(D64,3,1)</f>
+        <v>8</v>
+      </c>
+      <c r="O64" s="1" t="str">
+        <f t="shared" ref="O64" si="16">CONCATENATE("E",MID(D64,1,3))</f>
+        <v>EJ28</v>
+      </c>
+      <c r="P64" s="1" t="str">
+        <f t="shared" ref="P64" si="17">MID(D64,5,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E65" s="6">
+        <v>2.9E-5</v>
+      </c>
+      <c r="F65" s="1">
+        <v>23.8</v>
+      </c>
+      <c r="G65" s="1">
+        <v>21.2</v>
+      </c>
+      <c r="H65" s="1">
+        <v>16.8</v>
+      </c>
+      <c r="I65" s="1">
+        <v>13.4</v>
+      </c>
+      <c r="J65" s="1">
+        <v>11.9</v>
+      </c>
+      <c r="K65" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="L65" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="M65" s="1">
+        <v>6</v>
+      </c>
+      <c r="N65" s="1" t="str">
+        <f t="shared" ref="N65:N75" si="18">MID(D65,3,1)</f>
+        <v>8</v>
+      </c>
+      <c r="O65" s="1" t="str">
+        <f t="shared" ref="O65:O75" si="19">CONCATENATE("E",MID(D65,1,3))</f>
+        <v>EJ28</v>
+      </c>
+      <c r="P65" s="1" t="str">
+        <f t="shared" ref="P65:P75" si="20">MID(D65,5,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E66" s="6">
+        <v>4.6020000000000003E-5</v>
+      </c>
+      <c r="F66" s="1">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="G66" s="1">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="H66" s="1">
+        <v>26.7</v>
+      </c>
+      <c r="I66" s="1">
+        <v>21.2</v>
+      </c>
+      <c r="J66" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="K66" s="1">
+        <v>15</v>
+      </c>
+      <c r="L66" s="1">
+        <v>11.9</v>
+      </c>
+      <c r="M66" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="N66" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="O66" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>EJ28</v>
+      </c>
+      <c r="P66" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A67" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E67" s="6">
+        <v>1.9279999999999998E-5</v>
+      </c>
+      <c r="F67" s="1">
+        <v>15.8</v>
+      </c>
+      <c r="G67" s="1">
+        <v>14.1</v>
+      </c>
+      <c r="H67" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="I67" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="J67" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="K67" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="L67" s="1">
+        <v>5</v>
+      </c>
+      <c r="M67" s="1">
+        <v>4</v>
+      </c>
+      <c r="N67" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>9</v>
+      </c>
+      <c r="O67" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>EJ29</v>
+      </c>
+      <c r="P67" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A68" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E68" s="6">
+        <v>2.8030000000000001E-5</v>
+      </c>
+      <c r="F68" s="1">
+        <v>23</v>
+      </c>
+      <c r="G68" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="H68" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="I68" s="1">
+        <v>12.9</v>
+      </c>
+      <c r="J68" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="K68" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="L68" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="M68" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="N68" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>9</v>
+      </c>
+      <c r="O68" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>EJ29</v>
+      </c>
+      <c r="P68" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A69" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E69" s="6">
+        <v>4.4860000000000001E-5</v>
+      </c>
+      <c r="F69" s="1">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="G69" s="1">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="H69" s="1">
+        <v>26</v>
+      </c>
+      <c r="I69" s="1">
+        <v>20.7</v>
+      </c>
+      <c r="J69" s="1">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="K69" s="1">
+        <v>14.6</v>
+      </c>
+      <c r="L69" s="1">
+        <v>11.6</v>
+      </c>
+      <c r="M69" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="N69" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>9</v>
+      </c>
+      <c r="O69" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>EJ29</v>
+      </c>
+      <c r="P69" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E70" s="6">
+        <v>2.065E-5</v>
+      </c>
+      <c r="F70" s="1">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G70" s="1">
+        <v>15.1</v>
+      </c>
+      <c r="H70" s="1">
+        <v>12</v>
+      </c>
+      <c r="I70" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="J70" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="K70" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="L70" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="M70" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="N70" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="O70" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>EJ30</v>
+      </c>
+      <c r="P70" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A71" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E71" s="6">
+        <v>2.9E-5</v>
+      </c>
+      <c r="F71" s="1">
+        <v>23.8</v>
+      </c>
+      <c r="G71" s="1">
+        <v>21.2</v>
+      </c>
+      <c r="H71" s="1">
+        <v>16.8</v>
+      </c>
+      <c r="I71" s="1">
+        <v>13.4</v>
+      </c>
+      <c r="J71" s="1">
+        <v>11.9</v>
+      </c>
+      <c r="K71" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="L71" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="M71" s="1">
+        <v>6</v>
+      </c>
+      <c r="N71" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="O71" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>EJ30</v>
+      </c>
+      <c r="P71" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E72" s="6">
+        <v>4.6020000000000003E-5</v>
+      </c>
+      <c r="F72" s="1">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="G72" s="1">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="H72" s="1">
+        <v>26.7</v>
+      </c>
+      <c r="I72" s="1">
+        <v>21.2</v>
+      </c>
+      <c r="J72" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="K72" s="1">
+        <v>15</v>
+      </c>
+      <c r="L72" s="1">
+        <v>11.9</v>
+      </c>
+      <c r="M72" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="N72" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="O72" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>EJ30</v>
+      </c>
+      <c r="P72" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E73" s="6">
+        <v>2.2840000000000002E-5</v>
+      </c>
+      <c r="F73" s="1">
+        <v>18.7</v>
+      </c>
+      <c r="G73" s="1">
+        <v>16.7</v>
+      </c>
+      <c r="H73" s="1">
+        <v>13.3</v>
+      </c>
+      <c r="I73" s="1">
         <v>10.5</v>
       </c>
-      <c r="I32" s="4">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="J32" s="4">
-        <v>6.6</v>
-      </c>
-      <c r="K32" s="4">
-        <v>5.2</v>
-      </c>
-      <c r="L32" s="4">
+      <c r="J73" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="K73" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="L73" s="1">
+        <v>5.9</v>
+      </c>
+      <c r="M73" s="1">
         <v>4.7</v>
       </c>
-      <c r="M32" s="4">
-        <v>3.7</v>
-      </c>
-      <c r="N32" s="1" t="str">
-        <f>MID(D32,3,1)</f>
+      <c r="N73" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="O73" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>EJ31</v>
+      </c>
+      <c r="P73" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E74" s="6">
+        <v>3.0219999999999999E-5</v>
+      </c>
+      <c r="F74" s="1">
+        <v>24.8</v>
+      </c>
+      <c r="G74" s="1">
+        <v>22.1</v>
+      </c>
+      <c r="H74" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="I74" s="1">
+        <v>13.9</v>
+      </c>
+      <c r="J74" s="1">
+        <v>12.4</v>
+      </c>
+      <c r="K74" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="L74" s="1">
+        <v>7.8</v>
+      </c>
+      <c r="M74" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="N74" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="O74" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>EJ31</v>
+      </c>
+      <c r="P74" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E75" s="6">
+        <v>4.9889999999999998E-5</v>
+      </c>
+      <c r="F75" s="1">
+        <v>40.9</v>
+      </c>
+      <c r="G75" s="1">
+        <v>36.5</v>
+      </c>
+      <c r="H75" s="1">
+        <v>29</v>
+      </c>
+      <c r="I75" s="1">
+        <v>23</v>
+      </c>
+      <c r="J75" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="K75" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="L75" s="1">
+        <v>12.9</v>
+      </c>
+      <c r="M75" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="N75" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="O75" s="1" t="str">
+        <f t="shared" si="19"/>
+        <v>EJ31</v>
+      </c>
+      <c r="P75" s="1" t="str">
+        <f t="shared" si="20"/>
         <v>3</v>
-      </c>
-      <c r="O32" s="1" t="str">
-        <f>CONCATENATE("E",MID(D32,1,3))</f>
-        <v>EJ43</v>
-      </c>
-      <c r="P32" s="1" t="str">
-        <f>MID(D32,5,1)</f>
-        <v>4</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" s="1">
-        <v>1.5347000000000001E-4</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="4">
-        <v>17.7</v>
-      </c>
-      <c r="H33" s="4">
-        <v>15.8</v>
-      </c>
-      <c r="I33" s="4">
-        <v>12.5</v>
-      </c>
-      <c r="J33" s="4">
-        <v>9.9</v>
-      </c>
-      <c r="K33" s="4">
-        <v>7.9</v>
-      </c>
-      <c r="L33" s="4">
-        <v>7</v>
-      </c>
-      <c r="M33" s="4">
-        <v>5.6</v>
-      </c>
-      <c r="N33" s="1" t="str">
-        <f t="shared" ref="N33:N34" si="6">MID(D33,3,1)</f>
-        <v>3</v>
-      </c>
-      <c r="O33" s="1" t="str">
-        <f t="shared" ref="O33:O34" si="7">CONCATENATE("E",MID(D33,1,3))</f>
-        <v>EJ43</v>
-      </c>
-      <c r="P33" s="1" t="str">
-        <f t="shared" ref="P33:P34" si="8">MID(D33,5,1)</f>
-        <v>5</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="1">
-        <v>2.8881000000000002E-4</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I34" s="4">
-        <v>23.5</v>
-      </c>
-      <c r="J34" s="4">
-        <v>18.7</v>
-      </c>
-      <c r="K34" s="4">
-        <v>14.8</v>
-      </c>
-      <c r="L34" s="4">
-        <v>13.2</v>
-      </c>
-      <c r="M34" s="4">
-        <v>10.5</v>
-      </c>
-      <c r="N34" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
-      <c r="O34" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>EJ43</v>
-      </c>
-      <c r="P34" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="R34" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="S29" r:id="rId1"/>
+    <hyperlink ref="S29" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J4"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A3:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="5"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.15">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.15">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="5" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2411,11 +5056,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2493,7 +5138,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2513,7 +5158,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2533,7 +5178,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2553,7 +5198,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2573,7 +5218,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2593,7 +5238,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -2613,7 +5258,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>94</v>
       </c>
       <c r="C18" t="s">
@@ -2633,7 +5278,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2653,7 +5298,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2673,7 +5318,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -2693,7 +5338,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C23" t="s">
@@ -2773,7 +5418,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -2813,7 +5458,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>100</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -2873,7 +5518,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>107</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -2893,7 +5538,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>108</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -2913,7 +5558,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>109</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -2953,7 +5598,7 @@
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C38" t="s">
@@ -2995,23 +5640,23 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1"/>
-    <hyperlink ref="B13" r:id="rId2"/>
-    <hyperlink ref="B27" r:id="rId3"/>
-    <hyperlink ref="B19" r:id="rId4"/>
-    <hyperlink ref="B20" r:id="rId5"/>
-    <hyperlink ref="B21" r:id="rId6"/>
-    <hyperlink ref="B38" r:id="rId7"/>
-    <hyperlink ref="B23" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B12" r:id="rId10"/>
-    <hyperlink ref="B14" r:id="rId11"/>
-    <hyperlink ref="B16" r:id="rId12"/>
-    <hyperlink ref="B18" r:id="rId13"/>
-    <hyperlink ref="B30" r:id="rId14"/>
-    <hyperlink ref="B33" r:id="rId15"/>
-    <hyperlink ref="B34" r:id="rId16"/>
-    <hyperlink ref="B35" r:id="rId17"/>
+    <hyperlink ref="B15" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B27" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B19" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B20" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B21" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B38" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B23" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="B14" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="B18" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="B30" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="B33" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="B34" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="B35" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>